<commit_message>
Signed-off-by: LJ Freeket <email@example.com>
</commit_message>
<xml_diff>
--- a/config/config_vps_US_V2.xlsx
+++ b/config/config_vps_US_V2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="24225" windowHeight="12540"/>
+    <workbookView windowWidth="17895" windowHeight="11190"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="139">
   <si>
     <t>AppID_v1_adslock1-5</t>
   </si>
@@ -390,6 +390,9 @@
     <t>com.bubbleshootertree.bubbleclassis</t>
   </si>
   <si>
+    <t>https://play.google.com/store/apps/details?id=com.farmfruitheroes.legend.blockfever</t>
+  </si>
+  <si>
     <t>http://91.216.190.228/config/ad_full_2013.png</t>
   </si>
   <si>
@@ -397,6 +400,9 @@
   </si>
   <si>
     <t>http://91.216.190.228/config/native_ad_2013.png</t>
+  </si>
+  <si>
+    <t>com.farmfruitheroes.legend.blockfever</t>
   </si>
   <si>
     <t>https://play.google.com/store/apps/details?id=com.shoot.bubble.dragon.mania.offline</t>
@@ -467,14 +473,22 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
       <name val="宋体"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -488,20 +502,19 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF9C0006"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="1"/>
       <name val="宋体"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="宋体"/>
@@ -510,9 +523,32 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -526,9 +562,9 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -556,40 +592,10 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="13"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -603,7 +609,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -642,78 +648,168 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -726,97 +822,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -858,6 +864,35 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -869,6 +904,15 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -888,48 +932,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -945,13 +947,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -960,149 +966,149 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="13" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="34" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1475,7 +1481,7 @@
   <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27:D28"/>
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="6"/>
@@ -2118,19 +2124,19 @@
         <v>1</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>99</v>
+        <v>124</v>
       </c>
       <c r="D28" s="12" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E28" s="12" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="F28" s="12" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="G28" s="11" t="s">
-        <v>103</v>
+        <v>128</v>
       </c>
     </row>
     <row r="29" spans="1:7">
@@ -2141,19 +2147,19 @@
         <v>1</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="D29" s="12" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="E29" s="12" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="F29" s="12" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="G29" s="11" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -2164,19 +2170,19 @@
         <v>1</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="D30" s="12" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="E30" s="12" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="F30" s="12" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="G30" s="11" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -2265,27 +2271,27 @@
     <hyperlink ref="C26" r:id="rId82" display="https://play.google.com/store/apps/details?id=com.cs.assassin.hunter" tooltip="https://play.google.com/store/apps/details?id=com.cs.assassin.hunter"/>
     <hyperlink ref="E28" r:id="rId83" display="http://91.216.190.228/config/icon_2013.png" tooltip="http://91.216.190.228/config/icon_2013.png"/>
     <hyperlink ref="D28" r:id="rId84" display="http://91.216.190.228/config/ad_full_2013.png" tooltip="http://91.216.190.228/config/ad_full_2013.png"/>
-    <hyperlink ref="C28" r:id="rId70" display="https://play.google.com/store/apps/details?id=classic.bubble.shooter.game.bubbletower.legend" tooltip="https://play.google.com/store/apps/details?id=classic.bubble.shooter.game.bubbletower.legend"/>
-    <hyperlink ref="E30" r:id="rId85" display="http://91.216.190.251/config/icon_4001.png" tooltip="http://91.216.190.251/config/icon_4001.png"/>
-    <hyperlink ref="D30" r:id="rId86" display="http://91.216.190.251/config/ad_full_4001.png" tooltip="http://91.216.190.251/config/ad_full_4001.png"/>
-    <hyperlink ref="C30" r:id="rId87" display="https://play.google.com/store/apps/details?id=woodblock.woodoku.woodpuzzleblock" tooltip="https://play.google.com/store/apps/details?id=woodblock.woodoku.woodpuzzleblock"/>
-    <hyperlink ref="F28" r:id="rId88" display="http://91.216.190.228/config/native_ad_2013.png" tooltip="http://91.216.190.228/config/native_ad_2013.png"/>
-    <hyperlink ref="F30" r:id="rId89" display="http://91.216.190.251/config/native_ad_4001.png" tooltip="http://91.216.190.251/config/native_ad_4001.png"/>
-    <hyperlink ref="C5" r:id="rId90" display="https://play.google.com/store/apps/details?id=com.findthedifferences.policestory"/>
-    <hyperlink ref="C6" r:id="rId91" display="https://play.google.com/store/apps/details?id=com.solitaire.solitairespider"/>
-    <hyperlink ref="C7" r:id="rId92" display="https://play.google.com/store/apps/details?id=com.woodpuzzle.woodfinger"/>
-    <hyperlink ref="C8" r:id="rId93" display="https://play.google.com/store/apps/details?id=com.jewelbalst.kungfurabbitcrush"/>
-    <hyperlink ref="C9" r:id="rId94" display="https://play.google.com/store/apps/details?id=com.snakevsblock.snakevsvirus"/>
-    <hyperlink ref="C10" r:id="rId95" display="https://play.google.com/store/apps/details?id=com.twofortwo.dotsconnectlegend"/>
-    <hyperlink ref="C11" r:id="rId96" display="https://play.google.com/store/apps/details?id=com.hiddencitygame.finddifferences.fd"/>
-    <hyperlink ref="E29" r:id="rId97" display="http://91.216.190.228/config/icon_2014.png" tooltip="http://91.216.190.228/config/icon_2014.png"/>
-    <hyperlink ref="D29" r:id="rId98" display="http://91.216.190.228/config/ad_full_2014.png" tooltip="http://91.216.190.228/config/ad_full_2014.png"/>
-    <hyperlink ref="C29" r:id="rId99" display="https://play.google.com/store/apps/details?id=com.shoot.bubble.dragon.mania.offline" tooltip="https://play.google.com/store/apps/details?id=com.shoot.bubble.dragon.mania.offline"/>
-    <hyperlink ref="F29" r:id="rId100" display="http://91.216.190.228/config/native_ad_2014.png" tooltip="http://91.216.190.228/config/native_ad_2014.png"/>
-    <hyperlink ref="F27" r:id="rId101" display="http://91.216.190.228/config/native_ad_1010.png" tooltip="http://91.216.190.228/config/native_ad_1010.png"/>
-    <hyperlink ref="E27" r:id="rId102" display="http://91.216.190.228/config/icon_1010.png" tooltip="http://91.216.190.228/config/icon_1010.png"/>
-    <hyperlink ref="D27" r:id="rId103" display="http://91.216.190.228/config/ad_full_1010.png" tooltip="http://91.216.190.228/config/ad_full_1010.png"/>
-    <hyperlink ref="C27" r:id="rId104" display="https://play.google.com/store/apps/details?id=com.bubbleshootertree.bubbleclassis" tooltip="https://play.google.com/store/apps/details?id=com.bubbleshootertree.bubbleclassis"/>
+    <hyperlink ref="C28" r:id="rId85" display="https://play.google.com/store/apps/details?id=com.farmfruitheroes.legend.blockfever" tooltip="https://play.google.com/store/apps/details?id=com.farmfruitheroes.legend.blockfever"/>
+    <hyperlink ref="E30" r:id="rId86" display="http://91.216.190.251/config/icon_4001.png" tooltip="http://91.216.190.251/config/icon_4001.png"/>
+    <hyperlink ref="D30" r:id="rId87" display="http://91.216.190.251/config/ad_full_4001.png" tooltip="http://91.216.190.251/config/ad_full_4001.png"/>
+    <hyperlink ref="C30" r:id="rId88" display="https://play.google.com/store/apps/details?id=woodblock.woodoku.woodpuzzleblock" tooltip="https://play.google.com/store/apps/details?id=woodblock.woodoku.woodpuzzleblock"/>
+    <hyperlink ref="F28" r:id="rId89" display="http://91.216.190.228/config/native_ad_2013.png" tooltip="http://91.216.190.228/config/native_ad_2013.png"/>
+    <hyperlink ref="F30" r:id="rId90" display="http://91.216.190.251/config/native_ad_4001.png" tooltip="http://91.216.190.251/config/native_ad_4001.png"/>
+    <hyperlink ref="C5" r:id="rId91" display="https://play.google.com/store/apps/details?id=com.findthedifferences.policestory"/>
+    <hyperlink ref="C6" r:id="rId92" display="https://play.google.com/store/apps/details?id=com.solitaire.solitairespider"/>
+    <hyperlink ref="C7" r:id="rId93" display="https://play.google.com/store/apps/details?id=com.woodpuzzle.woodfinger"/>
+    <hyperlink ref="C8" r:id="rId94" display="https://play.google.com/store/apps/details?id=com.jewelbalst.kungfurabbitcrush"/>
+    <hyperlink ref="C9" r:id="rId95" display="https://play.google.com/store/apps/details?id=com.snakevsblock.snakevsvirus"/>
+    <hyperlink ref="C10" r:id="rId96" display="https://play.google.com/store/apps/details?id=com.twofortwo.dotsconnectlegend"/>
+    <hyperlink ref="C11" r:id="rId97" display="https://play.google.com/store/apps/details?id=com.hiddencitygame.finddifferences.fd"/>
+    <hyperlink ref="E29" r:id="rId98" display="http://91.216.190.228/config/icon_2014.png" tooltip="http://91.216.190.228/config/icon_2014.png"/>
+    <hyperlink ref="D29" r:id="rId99" display="http://91.216.190.228/config/ad_full_2014.png" tooltip="http://91.216.190.228/config/ad_full_2014.png"/>
+    <hyperlink ref="C29" r:id="rId100" display="https://play.google.com/store/apps/details?id=com.shoot.bubble.dragon.mania.offline" tooltip="https://play.google.com/store/apps/details?id=com.shoot.bubble.dragon.mania.offline"/>
+    <hyperlink ref="F29" r:id="rId101" display="http://91.216.190.228/config/native_ad_2014.png" tooltip="http://91.216.190.228/config/native_ad_2014.png"/>
+    <hyperlink ref="F27" r:id="rId102" display="http://91.216.190.228/config/native_ad_1010.png" tooltip="http://91.216.190.228/config/native_ad_1010.png"/>
+    <hyperlink ref="E27" r:id="rId103" display="http://91.216.190.228/config/icon_1010.png" tooltip="http://91.216.190.228/config/icon_1010.png"/>
+    <hyperlink ref="D27" r:id="rId104" display="http://91.216.190.228/config/ad_full_1010.png" tooltip="http://91.216.190.228/config/ad_full_1010.png"/>
+    <hyperlink ref="C27" r:id="rId105" display="https://play.google.com/store/apps/details?id=com.bubbleshootertree.bubbleclassis" tooltip="https://play.google.com/store/apps/details?id=com.bubbleshootertree.bubbleclassis"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.509027777777778" footer="0.509027777777778"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>